<commit_message>
new pages with testscripts
</commit_message>
<xml_diff>
--- a/src/test/resources/Opportunity.xlsx
+++ b/src/test/resources/Opportunity.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/582003e1f621abc3/Desktop/AutomateCRM/Automatesmb-9wood/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC104890F918537A5BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F891626-A041-41EA-B1C6-D4B2DB8C5BC8}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABDACC104890F918537A5BDE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ED137A3-05EB-427A-9971-81EB089A4F52}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Oppertunity" sheetId="1" r:id="rId1"/>
+    <sheet name="Opportunity" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -132,6 +132,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,7 +408,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>